<commit_message>
update testcase template for smart lighting
</commit_message>
<xml_diff>
--- a/testcases/template/智能照明.xlsx
+++ b/testcases/template/智能照明.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21210" windowHeight="10800" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19245" windowHeight="7440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="首页" sheetId="1" r:id="rId1"/>
@@ -21,15 +21,18 @@
   <definedNames>
     <definedName name="测试分析">OFFSET('[1]数据源 '!$A$1,0,0,COUNTA('[1]数据源 '!$A:$A),7)</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="9" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="105">
+  <si>
+    <t>StarRiver 智能zhaom测试用例</t>
+  </si>
   <si>
     <t>测试结果</t>
   </si>
@@ -118,12 +121,21 @@
     <t>Bug#</t>
   </si>
   <si>
+    <t>smartlight-statistics-001</t>
+  </si>
+  <si>
+    <t>统计</t>
+  </si>
+  <si>
     <t>计数项:测试编号</t>
   </si>
   <si>
     <t>列标签</t>
   </si>
   <si>
+    <t>smartlight-statistics-002</t>
+  </si>
+  <si>
     <t>行标签</t>
   </si>
   <si>
@@ -133,52 +145,30 @@
     <t>总计</t>
   </si>
   <si>
-    <t>StarRiver 智能zhaom测试用例</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>smartlight-statistics-001</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>smartlight-statistics-002</t>
-  </si>
-  <si>
     <t>smartlight-statistics-003</t>
   </si>
   <si>
     <t>smartlight-statistics-004</t>
   </si>
   <si>
-    <t>smartlight-statistics-005</t>
-  </si>
-  <si>
-    <t>smartlight-statistics-006</t>
-  </si>
-  <si>
-    <t>smartlight-statistics-007</t>
-  </si>
-  <si>
-    <t>smartlight-statistics-008</t>
-  </si>
-  <si>
-    <t>smartlight-statistics-009</t>
-  </si>
-  <si>
-    <t>统计</t>
-  </si>
-  <si>
-    <t>统计</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <t>地图</t>
+  </si>
+  <si>
+    <t>列表</t>
+  </si>
+  <si>
+    <t>控制</t>
   </si>
   <si>
     <t>smartlight-map-001</t>
-    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>smartlight-map-002</t>
   </si>
   <si>
+    <t>每点击某个域图标时，地图以选中域坐标作为原点，进入下一级缩放级别，同时显示当前级别下相关域或设备信息（按照坐标及可视范围计算后获得）</t>
+  </si>
+  <si>
     <t>smartlight-map-003</t>
   </si>
   <si>
@@ -188,61 +178,227 @@
     <t>smartlight-map-005</t>
   </si>
   <si>
-    <t>地图</t>
-  </si>
-  <si>
-    <t>地图</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>smartlight-list-001</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>列表</t>
-  </si>
-  <si>
-    <t>列表</t>
-    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>smartlight-list-002</t>
   </si>
   <si>
+    <t>smartlight-control-002</t>
+  </si>
+  <si>
+    <t>根据当前地图级别，显示对应级别域设备统计信息，以地图可见区域计算</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>进入统计页面，选择域</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>正确显示当前域能耗数据图及设备状态图</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>能耗统计周期选择：天</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>能耗统计周期选择：月</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>能耗图显示选择日期24小时数据图</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>能耗图显示选择日期当月每天能耗统计图</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>能耗图显示选择日期当年每月耗统计图</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>缩放地图</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>域显示及域级别跳转</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>smartlight-map-006</t>
+  </si>
+  <si>
+    <t>搜索列表：输入框输入搜索名称</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索域跳转</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索设备跳转</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 以选中域及对应级别作为中心显示地图及缩放级别
+2. 显示当前级别下，坐标范围内设置距离内设备或子域</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示满足条件的域和设备列表(并分页显示)，用不同图标表示，</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 地图以设备坐标缩放到到指定级别
+2. 显示设备图标及对应状态（在线/离线/故障）
+3. 显示设备属性界面</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>调光</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>smartlight-list-003</t>
   </si>
   <si>
     <t>smartlight-list-004</t>
   </si>
   <si>
+    <t>单灯控制器：地图坐标</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>能正确显示设备地图坐标</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>列表正确显示，可通过域和筛选条件显示正确结果及属性状态</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>网关：地图坐标</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>smartlight-list-005</t>
   </si>
   <si>
+    <t>smartlight-list-006</t>
+  </si>
+  <si>
+    <t>单灯控制器：开关控制</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>单灯控制器：调光</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 界面显示命令是否下发成功消息
+2. 观察测试设备状态发生变化</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>单灯控制器列表</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>网关列表</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>smartlight-control-001</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>smartlight-control-002</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间策略列表</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>正确显示配置好的时间策略列表及分组信息</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间策略状态</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 正确显示选中的策略状态（暂停/启用）
+2. 状态是互斥的，只能有一个当前可操作状态</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>smartlight-control-003</t>
   </si>
   <si>
+    <t>时间策略任务记录</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>正确显示当前策略执行任务列表信息</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>smartlight-control-004</t>
   </si>
   <si>
-    <t>控制</t>
-  </si>
-  <si>
-    <t>控制</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <t>时间策略操作：启用或暂停</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 界面显示命令是否下发成功消息
+2. 状态按钮更新状态</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>smartlight-control-005</t>
+  </si>
+  <si>
+    <t>smartlight-control-006</t>
+  </si>
+  <si>
+    <t>smartlight-control-007</t>
+  </si>
+  <si>
+    <t>smartlight-control-008</t>
+  </si>
+  <si>
+    <t>经纬度策略列表</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>经纬度策略状态</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>经纬度策略任务记录</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>经纬度策略操作：启用或暂停</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>唐跃元</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.0.2</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加测试用例</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,29 +411,14 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="8" tint="-0.249977111117893"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -285,7 +426,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -295,25 +436,52 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="9"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <family val="3"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="8" tint="-0.249977111117893"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -381,21 +549,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -412,26 +567,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -443,11 +586,207 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -468,9 +807,89 @@
       </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14993743705557422"/>
+          <bgColor theme="0" tint="-0.14990691854609822"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -504,7 +923,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[报表.xlsx]智能照明!数据透视表3</c:name>
+    <c:name>[智能照明.xlsx]智能照明!数据透视表3</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -649,124 +1068,6 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr lang="zh-CN" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="zh-CN"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="ctr"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="3"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:alpha val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:alpha val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr lang="zh-CN" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="zh-CN"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="ctr"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="4"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:alpha val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:alpha val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -784,7 +1085,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Success</c:v>
+                  <c:v>(空白)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -888,147 +1189,23 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-072F-4FF0-B1B2-5230BD674595}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>智能照明!$L$2:$L$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>(空白)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:alpha val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:alpha val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr lang="zh-CN" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="zh-CN"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>智能照明!$J$4:$J$9</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>(空白)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>统计</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>地图</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>列表</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>控制</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>智能照明!$L$4:$L$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EEC4-4450-A17B-182858BB066B}"/>
+              <c16:uniqueId val="{00000000-A904-42FB-BDB5-1118B4762A89}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1856,13 +2033,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>13970</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>318770</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>814070</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:colOff>725170</xdr:colOff>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>26670</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1870,7 +2047,7 @@
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1905,7 +2082,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="ccc" refreshedDate="43187.413095254633" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="65">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="ccc" refreshedDate="43192.548853935186" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F1048576" sheet="智能照明"/>
   </cacheSource>
@@ -1920,29 +2097,29 @@
         <s v="列表"/>
         <s v="控制"/>
         <m/>
+        <s v="故障管理" u="1"/>
+        <s v="统计:能耗" u="1"/>
+        <s v="单灯控制器" u="1"/>
+        <s v="资产统计" u="1"/>
+        <s v="资产模型" u="1"/>
+        <s v="网关" u="1"/>
+        <s v="图片属性" u="1"/>
+        <s v="视频属性" u="1"/>
         <s v="文字属性" u="1"/>
-        <s v="图片属性" u="1"/>
-        <s v="资产模型" u="1"/>
-        <s v="视频属性" u="1"/>
-        <s v="统计:能耗" u="1"/>
-        <s v="资产统计" u="1"/>
-        <s v="单灯控制器" u="1"/>
-        <s v="网关" u="1"/>
-        <s v="故障管理" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="测试目标/步骤" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+      <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="期望" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+      <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="测试结果" numFmtId="0">
-      <sharedItems containsBlank="1" count="4">
-        <s v="Success"/>
+      <sharedItems containsNonDate="0" containsBlank="1" count="4">
         <m/>
+        <s v="Success" u="1"/>
+        <s v="Failed" u="1"/>
         <s v="Skip" u="1"/>
-        <s v="Failed" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Bug#" numFmtId="0">
@@ -1958,189 +2135,197 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="65">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="64">
   <r>
     <s v="smartlight-statistics-001"/>
     <x v="0"/>
-    <m/>
-    <m/>
+    <s v="进入统计页面，选择域"/>
+    <s v="正确显示当前域能耗数据图及设备状态图"/>
     <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-statistics-002"/>
     <x v="0"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="能耗统计周期选择：天"/>
+    <s v="能耗图显示选择日期24小时数据图"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-statistics-003"/>
     <x v="0"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="能耗统计周期选择：月"/>
+    <s v="能耗图显示选择日期当月每天能耗统计图"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-statistics-004"/>
     <x v="0"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="smartlight-statistics-005"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="smartlight-statistics-006"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="smartlight-statistics-007"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="smartlight-statistics-008"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="smartlight-statistics-009"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="能耗统计周期选择：天"/>
+    <s v="能耗图显示选择日期当年每月耗统计图"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-map-001"/>
     <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="缩放地图"/>
+    <s v="根据当前地图级别，显示对应级别域设备统计信息，以地图可见区域计算"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-map-002"/>
     <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="域显示及域级别跳转"/>
+    <s v="每点击某个域图标时，地图以选中域坐标作为原点，进入下一级缩放级别，同时显示当前级别下相关域或设备信息（按照坐标及可视范围计算后获得）"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-map-003"/>
     <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="搜索列表：输入框输入搜索名称"/>
+    <s v="显示满足条件的域和设备列表(并分页显示)，用不同图标表示，"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-map-004"/>
     <x v="1"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="搜索域跳转"/>
+    <s v="1. 以选中域及对应级别作为中心显示地图及缩放级别_x000a_2. 显示当前级别下，坐标范围内设置距离内设备或子域"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-map-005"/>
     <x v="1"/>
-    <m/>
-    <m/>
+    <s v="搜索设备跳转"/>
+    <s v="1. 地图以设备坐标缩放到到指定级别_x000a_2. 显示设备图标及对应状态（在线/离线/故障）_x000a_3. 显示设备属性界面"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="smartlight-map-006"/>
     <x v="1"/>
+    <s v="调光"/>
+    <s v="1. 界面显示命令是否下发成功消息_x000a_2. 观察测试设备状态发生变化"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-list-001"/>
     <x v="2"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="单灯控制器列表"/>
+    <s v="列表正确显示，可通过域和筛选条件显示正确结果及属性状态"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-list-002"/>
     <x v="2"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="单灯控制器：地图坐标"/>
+    <s v="能正确显示设备地图坐标"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-list-003"/>
     <x v="2"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="单灯控制器：开关控制"/>
+    <s v="1. 界面显示命令是否下发成功消息_x000a_2. 观察测试设备状态发生变化"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-list-004"/>
     <x v="2"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="单灯控制器：调光"/>
+    <s v="1. 界面显示命令是否下发成功消息_x000a_2. 观察测试设备状态发生变化"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-list-005"/>
     <x v="2"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="网关列表"/>
+    <s v="列表正确显示，可通过域和筛选条件显示正确结果及属性状态"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="smartlight-list-006"/>
+    <x v="2"/>
+    <s v="网关：地图坐标"/>
+    <s v="能正确显示设备地图坐标"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-control-001"/>
     <x v="3"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="时间策略列表"/>
+    <s v="正确显示配置好的时间策略列表及分组信息"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-control-002"/>
     <x v="3"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="时间策略状态"/>
+    <s v="1. 正确显示选中的策略状态（暂停/启用）_x000a_2. 状态是互斥的，只能有一个当前可操作状态"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-control-003"/>
     <x v="3"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="时间策略任务记录"/>
+    <s v="正确显示当前策略执行任务列表信息"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
     <s v="smartlight-control-004"/>
     <x v="3"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <s v="时间策略操作：启用或暂停"/>
+    <s v="1. 界面显示命令是否下发成功消息_x000a_2. 状态按钮更新状态"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="smartlight-control-005"/>
+    <x v="3"/>
+    <s v="经纬度策略列表"/>
+    <s v="正确显示配置好的时间策略列表及分组信息"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="smartlight-control-006"/>
+    <x v="3"/>
+    <s v="经纬度策略状态"/>
+    <s v="1. 正确显示选中的策略状态（暂停/启用）_x000a_2. 状态是互斥的，只能有一个当前可操作状态"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="smartlight-control-007"/>
+    <x v="3"/>
+    <s v="经纬度策略任务记录"/>
+    <s v="正确显示当前策略执行任务列表信息"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="smartlight-control-008"/>
+    <x v="3"/>
+    <s v="经纬度策略操作：启用或暂停"/>
+    <s v="1. 界面显示命令是否下发成功消息_x000a_2. 状态按钮更新状态"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2148,7 +2333,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2156,7 +2341,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2164,7 +2349,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2172,7 +2357,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2180,7 +2365,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2188,7 +2373,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2196,7 +2381,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2204,7 +2389,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2212,7 +2397,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2220,7 +2405,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2228,7 +2413,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2236,7 +2421,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2244,7 +2429,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2252,7 +2437,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2260,7 +2445,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2268,7 +2453,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2276,7 +2461,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2284,7 +2469,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2292,7 +2477,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2300,7 +2485,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2308,7 +2493,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2316,7 +2501,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2324,7 +2509,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2332,7 +2517,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2340,7 +2525,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2348,7 +2533,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2356,7 +2541,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2364,7 +2549,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2372,7 +2557,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2380,7 +2565,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2388,7 +2573,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2396,7 +2581,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2404,7 +2589,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2412,7 +2597,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2420,7 +2605,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2428,7 +2613,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2436,7 +2621,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2444,7 +2629,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2452,7 +2637,7 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
   <r>
@@ -2460,45 +2645,29 @@
     <x v="4"/>
     <m/>
     <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="4"/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="4"/>
-    <m/>
-    <m/>
-    <x v="1"/>
+    <x v="0"/>
     <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="J2:M9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表3" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="J2:L9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0">
       <items count="15">
-        <item sd="0" m="1" x="5"/>
+        <item sd="0" m="1" x="13"/>
         <item sd="0" x="4"/>
-        <item sd="0" m="1" x="6"/>
-        <item sd="0" m="1" x="8"/>
+        <item sd="0" m="1" x="11"/>
+        <item sd="0" m="1" x="12"/>
+        <item m="1" x="9"/>
+        <item m="1" x="8"/>
+        <item m="1" x="10"/>
         <item m="1" x="7"/>
-        <item m="1" x="10"/>
-        <item m="1" x="12"/>
-        <item m="1" x="11"/>
-        <item m="1" x="13"/>
-        <item m="1" x="9"/>
+        <item m="1" x="5"/>
+        <item m="1" x="6"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -2510,10 +2679,10 @@
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
       <items count="5">
+        <item m="1" x="2"/>
         <item m="1" x="3"/>
-        <item m="1" x="2"/>
+        <item m="1" x="1"/>
         <item x="0"/>
-        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2545,10 +2714,7 @@
   <colFields count="1">
     <field x="4"/>
   </colFields>
-  <colItems count="3">
-    <i>
-      <x v="2"/>
-    </i>
+  <colItems count="2">
     <i>
       <x v="3"/>
     </i>
@@ -2559,7 +2725,47 @@
   <dataFields count="1">
     <dataField name="计数项:测试编号" fld="0" subtotal="count" baseField="1" baseItem="0"/>
   </dataFields>
-  <chartFormats count="5">
+  <formats count="10">
+    <format dxfId="32">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="31">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="30">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="29">
+      <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="28">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="27">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="26">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="24">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="23">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="3">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -2567,7 +2773,7 @@
             <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="0"/>
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -2579,7 +2785,7 @@
             <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="1"/>
+            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
@@ -2591,27 +2797,6 @@
             <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
@@ -2891,7 +3076,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2904,168 +3089,176 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="F1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="23"/>
+      <c r="I1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="13">
+      <c r="I2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="8">
         <v>43179</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
+      <c r="A3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="13">
+      <c r="I3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="8">
         <v>43182</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="I4" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="J4" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
+      <c r="A5" s="3">
         <v>43187</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="D5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="I5" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="J5" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="11"/>
+      <c r="A6" s="3">
+        <v>43192</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="11"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3073,7 +3266,7 @@
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="A3:D3"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -3081,626 +3274,832 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M65"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.25" customWidth="1"/>
-    <col min="2" max="2" width="7.75" customWidth="1"/>
-    <col min="3" max="3" width="45.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="11.25" customWidth="1"/>
-    <col min="7" max="7" width="18.375" customWidth="1"/>
-    <col min="8" max="9" width="4" customWidth="1"/>
-    <col min="10" max="10" width="15.625"/>
-    <col min="11" max="11" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.375"/>
-    <col min="15" max="15" width="5.125"/>
-    <col min="16" max="16" width="10.875" customWidth="1"/>
-    <col min="17" max="17" width="11" customWidth="1"/>
-    <col min="18" max="18" width="9.375" customWidth="1"/>
-    <col min="19" max="19" width="12.375" customWidth="1"/>
-    <col min="20" max="20" width="10.875" customWidth="1"/>
-    <col min="21" max="21" width="5.25" customWidth="1"/>
+    <col min="1" max="1" width="22.75" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.75" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.25" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.75" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.25" style="15" customWidth="1"/>
+    <col min="8" max="9" width="4" style="15" customWidth="1"/>
+    <col min="10" max="10" width="15.875" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.375" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.125" style="15"/>
+    <col min="16" max="16" width="10.875" style="15" customWidth="1"/>
+    <col min="17" max="17" width="11" style="15" customWidth="1"/>
+    <col min="18" max="18" width="9.375" style="15" customWidth="1"/>
+    <col min="19" max="19" width="12.375" style="15" customWidth="1"/>
+    <col min="20" max="20" width="10.875" style="15" customWidth="1"/>
+    <col min="21" max="21" width="5.25" style="15" customWidth="1"/>
+    <col min="22" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="J2" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2"/>
+      <c r="N2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="J3" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3"/>
+      <c r="N3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="J4" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4"/>
+      <c r="N4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="19"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="J5" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="22">
+        <v>4</v>
+      </c>
+      <c r="L5" s="22">
+        <v>4</v>
+      </c>
+      <c r="M5"/>
+      <c r="N5"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="J6" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="22">
+        <v>6</v>
+      </c>
+      <c r="L6" s="22">
+        <v>6</v>
+      </c>
+      <c r="M6"/>
+      <c r="N6"/>
+    </row>
+    <row r="7" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="J7" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="22">
+        <v>6</v>
+      </c>
+      <c r="L7" s="22">
+        <v>6</v>
+      </c>
+      <c r="M7"/>
+      <c r="N7"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="J8" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="22">
+        <v>8</v>
+      </c>
+      <c r="L8" s="22">
+        <v>8</v>
+      </c>
+      <c r="M8"/>
+      <c r="N8"/>
+    </row>
+    <row r="9" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="J9" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="22">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17"/>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-      <c r="J3" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
-      <c r="J4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
-      <c r="J5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" s="19">
-        <v>1</v>
-      </c>
-      <c r="L5" s="19">
-        <v>8</v>
-      </c>
-      <c r="M5" s="19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="J6" s="5" t="s">
+      <c r="L9" s="22">
+        <v>24</v>
+      </c>
+      <c r="M9"/>
+      <c r="N9"/>
+    </row>
+    <row r="10" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="19"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+    </row>
+    <row r="14" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+    </row>
+    <row r="15" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+    </row>
+    <row r="19" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19">
-        <v>5</v>
-      </c>
-      <c r="M6" s="19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
-      <c r="J7" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19">
-        <v>5</v>
-      </c>
-      <c r="M7" s="19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17"/>
-      <c r="J8" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19">
-        <v>4</v>
-      </c>
-      <c r="M8" s="19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="B19" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
-      <c r="J9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="19">
-        <v>1</v>
-      </c>
-      <c r="L9" s="19">
-        <v>22</v>
-      </c>
-      <c r="M9" s="19">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="2"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="2"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="2"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="2"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="2"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="2"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="2"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="2"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
+      <c r="C19" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+    </row>
+    <row r="21" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="19"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+    </row>
+    <row r="23" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+    </row>
+    <row r="25" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="16"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="16"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="16"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="16"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="16"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="16"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="16"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="16"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="16"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="16"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="16"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="16"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="16"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+    </row>
+    <row r="39" spans="1:7" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A39" s="16"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="23"/>
+    </row>
+    <row r="40" spans="1:7" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A40" s="16"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="23"/>
+    </row>
+    <row r="41" spans="1:7" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A41" s="16"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="23"/>
+    </row>
+    <row r="42" spans="1:7" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A42" s="16"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="23"/>
+    </row>
+    <row r="43" spans="1:7" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A43" s="16"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="23"/>
+    </row>
+    <row r="44" spans="1:7" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A44" s="16"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="23"/>
+    </row>
+    <row r="45" spans="1:7" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A45" s="16"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="23"/>
+    </row>
+    <row r="46" spans="1:7" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A46" s="16"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="23"/>
+    </row>
+    <row r="47" spans="1:7" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A47" s="16"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="23"/>
+    </row>
+    <row r="48" spans="1:7" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A48" s="16"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="23"/>
+    </row>
+    <row r="49" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A49" s="16"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="23"/>
+    </row>
+    <row r="50" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A50" s="16"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="23"/>
+    </row>
+    <row r="51" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A51" s="16"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="23"/>
+    </row>
+    <row r="52" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A52" s="16"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="23"/>
+    </row>
+    <row r="53" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A53" s="16"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="23"/>
+    </row>
+    <row r="54" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A54" s="16"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="23"/>
+    </row>
+    <row r="55" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A55" s="16"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="23"/>
+    </row>
+    <row r="56" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A56" s="16"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="23"/>
+    </row>
+    <row r="57" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A57" s="24"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+    </row>
+    <row r="58" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A58" s="24"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+    </row>
+    <row r="59" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A59" s="24"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+    </row>
+    <row r="60" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A60" s="24"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+    </row>
+    <row r="61" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A61" s="24"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+    </row>
+    <row r="62" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A62" s="24"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+    </row>
+    <row r="63" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A63" s="24"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="23"/>
+    </row>
+    <row r="64" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A64" s="24"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
       <formula>"Skip"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>"Success"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3714,7 +4113,7 @@
           <x14:formula1>
             <xm:f>首页!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E1532</xm:sqref>
+          <xm:sqref>E1:E1531</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>